<commit_message>
auto eval + pdf + readme
</commit_message>
<xml_diff>
--- a/Atelier3/Auto éval.xlsx
+++ b/Atelier3/Auto éval.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guizo\OneDrive\Bureau\Codage\CPE\S8\ASI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guizo\OneDrive\Bureau\Codage\CPE\S8\ASI\ASI_CPE\Atelier3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB531B6F-6F2B-4927-8597-5A6636BB6C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400BBE4D-6A6E-4123-BB8E-6C6D663F14FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,25 +509,47 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -573,28 +595,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF00B050"/>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -811,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L56" sqref="L56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P52" sqref="P52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.05" customHeight="1"/>
@@ -825,31 +825,31 @@
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" customHeight="1">
       <c r="C1" s="1"/>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="17" t="s">
+      <c r="H1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="17" t="s">
+      <c r="K1" s="22"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="18"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="20" t="s">
+      <c r="N1" s="22"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="22"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="18"/>
       <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:19" ht="14.25" customHeight="1">
@@ -919,10 +919,10 @@
       <c r="R3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" customHeight="1">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="9">
         <v>0.25</v>
       </c>
@@ -973,11 +973,11 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -993,10 +993,10 @@
     </row>
     <row r="6" spans="1:19" ht="14.25" customHeight="1">
       <c r="A6" s="6"/>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -1016,7 +1016,7 @@
       <c r="C7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="15" t="s">
@@ -1062,7 +1062,7 @@
       <c r="C8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="15" t="s">
@@ -1154,14 +1154,14 @@
       <c r="C10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>14</v>
@@ -1170,7 +1170,7 @@
         <v>14</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J10" s="13" t="s">
         <v>14</v>
@@ -1216,7 +1216,7 @@
         <v>19</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J11" s="13" t="s">
         <v>12</v>
@@ -1262,7 +1262,7 @@
         <v>19</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J12" s="13" t="s">
         <v>14</v>
@@ -1354,7 +1354,7 @@
         <v>17</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J14" s="13" t="s">
         <v>17</v>
@@ -1400,7 +1400,7 @@
         <v>17</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J15" s="13" t="s">
         <v>17</v>
@@ -1464,7 +1464,7 @@
         <v>17</v>
       </c>
       <c r="O16" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
@@ -1529,7 +1529,7 @@
         <v>17</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>17</v>
@@ -1897,7 +1897,7 @@
         <v>14</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>12</v>
@@ -1943,7 +1943,7 @@
         <v>14</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>14</v>
@@ -1961,7 +1961,7 @@
         <v>19</v>
       </c>
       <c r="L27" s="13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="M27" s="13" t="s">
         <v>14</v>
@@ -1989,7 +1989,7 @@
         <v>14</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G28" s="13" t="s">
         <v>14</v>
@@ -2007,7 +2007,7 @@
         <v>19</v>
       </c>
       <c r="L28" s="13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="M28" s="13" t="s">
         <v>14</v>
@@ -2035,7 +2035,7 @@
         <v>14</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>14</v>
@@ -2053,7 +2053,7 @@
         <v>19</v>
       </c>
       <c r="L29" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M29" s="13" t="s">
         <v>14</v>
@@ -2081,7 +2081,7 @@
         <v>14</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G30" s="13" t="s">
         <v>14</v>
@@ -2099,7 +2099,7 @@
         <v>19</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M30" s="13" t="s">
         <v>14</v>
@@ -2127,7 +2127,7 @@
         <v>39</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>39</v>
@@ -2145,7 +2145,7 @@
         <v>17</v>
       </c>
       <c r="L31" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="M31" s="13" t="s">
         <v>17</v>
@@ -2219,7 +2219,7 @@
         <v>39</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G33" s="13" t="s">
         <v>14</v>
@@ -2237,7 +2237,7 @@
         <v>39</v>
       </c>
       <c r="L33" s="13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M33" s="13" t="s">
         <v>39</v>
@@ -2265,7 +2265,7 @@
         <v>39</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G34" s="13" t="s">
         <v>17</v>
@@ -2283,7 +2283,7 @@
         <v>39</v>
       </c>
       <c r="L34" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M34" s="13" t="s">
         <v>39</v>
@@ -2311,7 +2311,7 @@
         <v>17</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>17</v>
@@ -2346,10 +2346,10 @@
     </row>
     <row r="36" spans="1:18" ht="14.25" customHeight="1">
       <c r="A36" s="6"/>
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="22"/>
+      <c r="C36" s="18"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
@@ -2462,22 +2462,22 @@
         <v>47</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="I39" s="13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="J39" s="13" t="s">
         <v>12</v>
@@ -2508,22 +2508,22 @@
         <v>48</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="J40" s="13" t="s">
         <v>12</v>
@@ -2535,13 +2535,13 @@
         <v>12</v>
       </c>
       <c r="M40" s="13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="N40" s="13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="O40" s="13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="P40" s="14"/>
       <c r="Q40" s="14"/>
@@ -2581,13 +2581,13 @@
         <v>12</v>
       </c>
       <c r="M41" s="13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="N41" s="13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="O41" s="13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="P41" s="14"/>
       <c r="Q41" s="14"/>
@@ -2627,13 +2627,13 @@
         <v>12</v>
       </c>
       <c r="M42" s="13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="N42" s="13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="O42" s="13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="P42" s="14"/>
       <c r="Q42" s="14"/>
@@ -2710,13 +2710,13 @@
         <v>14</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="L44" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="M44" s="13" t="s">
         <v>39</v>
@@ -2756,13 +2756,13 @@
         <v>14</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L45" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M45" s="13" t="s">
         <v>14</v>
@@ -2787,10 +2787,10 @@
         <v>19</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G46" s="13" t="s">
         <v>14</v>
@@ -2802,13 +2802,13 @@
         <v>14</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K46" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L46" s="13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="M46" s="13" t="s">
         <v>14</v>
@@ -2833,10 +2833,10 @@
         <v>19</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G47" s="13" t="s">
         <v>14</v>
@@ -2845,7 +2845,7 @@
         <v>14</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J47" s="13" t="s">
         <v>19</v>
@@ -2854,7 +2854,7 @@
         <v>19</v>
       </c>
       <c r="L47" s="13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="M47" s="13" t="s">
         <v>14</v>
@@ -2863,7 +2863,7 @@
         <v>14</v>
       </c>
       <c r="O47" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="P47" s="14"/>
       <c r="Q47" s="14"/>
@@ -2882,7 +2882,7 @@
         <v>17</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G48" s="13" t="s">
         <v>14</v>
@@ -2891,7 +2891,7 @@
         <v>14</v>
       </c>
       <c r="I48" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J48" s="13" t="s">
         <v>17</v>
@@ -2900,7 +2900,7 @@
         <v>17</v>
       </c>
       <c r="L48" s="13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="M48" s="13" t="s">
         <v>17</v>
@@ -2909,7 +2909,7 @@
         <v>17</v>
       </c>
       <c r="O48" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="P48" s="14"/>
       <c r="Q48" s="14"/>
@@ -2928,7 +2928,7 @@
         <v>39</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="G49" s="13" t="s">
         <v>14</v>
@@ -2937,7 +2937,7 @@
         <v>14</v>
       </c>
       <c r="I49" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J49" s="13" t="s">
         <v>17</v>
@@ -2946,7 +2946,7 @@
         <v>17</v>
       </c>
       <c r="L49" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M49" s="13" t="s">
         <v>17</v>
@@ -2955,7 +2955,7 @@
         <v>17</v>
       </c>
       <c r="O49" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="P49" s="14"/>
       <c r="Q49" s="14"/>
@@ -2974,7 +2974,7 @@
         <v>39</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="G50" s="13" t="s">
         <v>39</v>
@@ -2983,7 +2983,7 @@
         <v>39</v>
       </c>
       <c r="I50" s="13" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="J50" s="13" t="s">
         <v>39</v>
@@ -2992,7 +2992,7 @@
         <v>39</v>
       </c>
       <c r="L50" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M50" s="13" t="s">
         <v>17</v>
@@ -3029,7 +3029,7 @@
         <v>39</v>
       </c>
       <c r="I51" s="13" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="J51" s="13" t="s">
         <v>39</v>
@@ -3038,7 +3038,7 @@
         <v>39</v>
       </c>
       <c r="L51" s="13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M51" s="13" t="s">
         <v>17</v>
@@ -3075,7 +3075,7 @@
         <v>39</v>
       </c>
       <c r="I52" s="13" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="J52" s="13" t="s">
         <v>39</v>
@@ -3121,7 +3121,7 @@
         <v>39</v>
       </c>
       <c r="I53" s="13" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="J53" s="13" t="s">
         <v>39</v>
@@ -3130,7 +3130,7 @@
         <v>39</v>
       </c>
       <c r="L53" s="13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M53" s="13" t="s">
         <v>17</v>
@@ -3158,7 +3158,7 @@
         <v>17</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="G54" s="16" t="s">
         <v>39</v>
@@ -3176,16 +3176,16 @@
         <v>39</v>
       </c>
       <c r="L54" s="16" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="M54" s="16" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="N54" s="16" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="O54" s="16" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="P54" s="14"/>
       <c r="Q54" s="14"/>
@@ -6031,43 +6031,43 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D37:O54 D7:O35">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:O54 D7:O35">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"AB"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:O54 D7:O35">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"B"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:O54 D7:O35">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"C"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:O54 D7:O35">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:O54 D7:O35">
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6096,12 +6096,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:R4">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:R4">
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6111,8 +6111,8 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>